<commit_message>
Added Southern Subtropical Front to all plots.
</commit_message>
<xml_diff>
--- a/Table 2 - SurfaceVariables/Table-X-SurfaceVariables.xlsx
+++ b/Table 2 - SurfaceVariables/Table-X-SurfaceVariables.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26920" windowHeight="14960" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14960" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Frontal Locations" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="82">
   <si>
     <t>Year</t>
   </si>
@@ -250,6 +250,48 @@
   <si>
     <t>N:P Ratio</t>
   </si>
+  <si>
+    <t>STG 27°-28°N index</t>
+  </si>
+  <si>
+    <t>6-10</t>
+  </si>
+  <si>
+    <t>4-6</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>SSTF 19.5°-20.5° index</t>
+  </si>
+  <si>
+    <t>SSTF Latitude</t>
+  </si>
+  <si>
+    <t>28°-29.25°N</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>30.5°-31.75°N</t>
+  </si>
+  <si>
+    <t>20-24</t>
+  </si>
+  <si>
+    <t>9-13</t>
+  </si>
+  <si>
+    <t>15-20</t>
+  </si>
+  <si>
+    <t>29.75°-31°N</t>
+  </si>
+  <si>
+    <t>6-8</t>
+  </si>
 </sst>
 </file>
 
@@ -258,7 +300,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -298,13 +340,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -345,7 +399,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -403,8 +457,41 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -426,9 +513,6 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -436,8 +520,25 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="57"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="57" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="57" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="57" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="16" fontId="5" fillId="2" borderId="0" xfId="57" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="90">
+    <cellStyle name="Bad" xfId="57" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -466,6 +567,22 @@
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -494,6 +611,22 @@
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -832,17 +965,17 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:9" ht="16">
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
       <c r="F1" s="4"/>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
@@ -942,17 +1075,17 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="16">
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="2" t="s">
@@ -1094,12 +1227,12 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
@@ -1145,427 +1278,529 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23:H25"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.1640625" customWidth="1"/>
-    <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="3" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.1640625" customWidth="1"/>
+    <col min="9" max="9" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12">
+      <c r="A1" s="15" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="3" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="D2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="F2" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="G2" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="H2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="I2" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="J2" s="16" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="E3" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" t="s">
+      <c r="F3" s="17"/>
+      <c r="G3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="I3" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" s="15"/>
+      <c r="K3" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
+    <row r="4" spans="1:12">
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="7">
+      <c r="E4" s="18">
         <v>39893</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" t="s">
+      <c r="F4" s="18"/>
+      <c r="G4" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="I4" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" s="15"/>
+      <c r="K4" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
+    <row r="5" spans="1:12">
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="E5" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" t="s">
+      <c r="F5" s="19"/>
+      <c r="G5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="I5" s="17" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="12" t="s">
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="11" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="12" t="s">
+      <c r="B7" s="11"/>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="11" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="B8" s="11"/>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="J9" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
-      <c r="A10" t="s">
+    <row r="10" spans="1:12">
+      <c r="A10" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" t="s">
         <v>46</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D10" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="E10" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" t="s">
+      <c r="F10" s="6"/>
+      <c r="G10" t="s">
         <v>8</v>
       </c>
-      <c r="F10" t="s">
+      <c r="H10" t="s">
         <v>43</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="I10" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
-      <c r="A11" t="s">
+    <row r="11" spans="1:12">
+      <c r="A11" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" t="s">
         <v>48</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D11" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="7">
+      <c r="E11" s="7">
         <v>39893</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" t="s">
+      <c r="F11" s="7"/>
+      <c r="G11" t="s">
         <v>38</v>
       </c>
-      <c r="F11" t="s">
+      <c r="H11" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="I11" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
-      <c r="A12" t="s">
+    <row r="12" spans="1:12">
+      <c r="A12" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" t="s">
         <v>50</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D12" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="E12" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" t="s">
+      <c r="F12" s="8"/>
+      <c r="G12" t="s">
         <v>9</v>
       </c>
-      <c r="F12" t="s">
+      <c r="H12" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="I12" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
-      <c r="A15" s="12" t="s">
+    <row r="15" spans="1:12">
+      <c r="A15" s="11" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="B15" s="11"/>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="G16" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="H16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="I16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="J16" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="11" t="s">
+    <row r="17" spans="1:10">
+      <c r="A17" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B17" t="s">
+      <c r="D17" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="E17" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="6"/>
-      <c r="E17" t="s">
+      <c r="F17" s="6"/>
+      <c r="G17" t="s">
         <v>51</v>
       </c>
-      <c r="F17" t="s">
+      <c r="H17" t="s">
         <v>43</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="I17" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:10">
       <c r="A18" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B18" t="s">
+      <c r="D18" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="7">
+      <c r="E18" s="7">
         <v>39893</v>
       </c>
-      <c r="D18" s="7"/>
-      <c r="E18" t="s">
+      <c r="F18" s="7"/>
+      <c r="G18" t="s">
         <v>55</v>
       </c>
-      <c r="F18" t="s">
+      <c r="H18" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="I18" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:10">
       <c r="A19" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B19" t="s">
+      <c r="D19" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="E19" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="10" t="s">
+      <c r="F19" s="8"/>
+      <c r="G19" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="F19" t="s">
+      <c r="H19" t="s">
         <v>42</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="I19" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="12" t="s">
+    <row r="21" spans="1:10">
+      <c r="A21" s="11" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="B21" s="11"/>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="E22" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="F22" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="G22" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="H22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="I22" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="J22" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="11" t="s">
+    <row r="23" spans="1:10">
+      <c r="A23" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B23" t="s">
+      <c r="D23" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="E23" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="13">
+      <c r="F23" s="12">
         <v>14.9964190582785</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="G23" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F23" t="s">
+      <c r="H23" t="s">
         <v>43</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="I23" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="H23" s="14">
+      <c r="J23" s="13">
         <v>16.921301270796899</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:10">
       <c r="A24" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="7">
+      <c r="E24" s="7">
         <v>39893</v>
       </c>
-      <c r="D24" s="13">
+      <c r="F24" s="12">
         <v>14.481906897791999</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="G24" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="F24" t="s">
+      <c r="H24" t="s">
         <v>39</v>
       </c>
-      <c r="G24" s="8" t="s">
+      <c r="I24" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="H24" s="14">
+      <c r="J24" s="13">
         <v>14.734212145307801</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:10">
       <c r="A25" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B25" t="s">
+      <c r="D25" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="E25" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="13">
+      <c r="F25" s="12">
         <v>14.2431107560074</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="G25" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="F25" t="s">
+      <c r="H25" t="s">
         <v>42</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="I25" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="H25" s="14">
+      <c r="J25" s="13">
         <v>14.5142202430478</v>
       </c>
     </row>

</xml_diff>